<commit_message>
Made progress on updating codebooks. Not done yet
</commit_message>
<xml_diff>
--- a/data/metaware_csv_codebooks.xlsx
+++ b/data/metaware_csv_codebooks.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas Coles work\Documents\experimentology_coles-fork\metaware\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ncole\Documents\GitHub\metaware\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49FDBFA0-BC6F-475D-9A66-D0A311AA9952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18790ADE-9169-4F34-820F-667278FE2C6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="17385" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metaware_VigCombined.csv" sheetId="3" r:id="rId1"/>
     <sheet name="metaware_SurvData_raw.csv" sheetId="2" r:id="rId2"/>
-    <sheet name="metaware_meta_clean.csv" sheetId="4" r:id="rId3"/>
-    <sheet name="metaware_replication_clean.csv" sheetId="5" r:id="rId4"/>
+    <sheet name="metaware_SurvData2_raw.csv " sheetId="6" r:id="rId3"/>
+    <sheet name="metaware_meta_clean.csv" sheetId="4" r:id="rId4"/>
+    <sheet name="metaware_replication_clean.csv" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="258">
   <si>
     <t>Variable</t>
   </si>
@@ -1244,6 +1245,51 @@
 native_pacific_islander = answered "Native Hawaiian or Other Pacific Islander"
 other = answered "other" or chose multiple ethnicities
 unknown = did not answer</t>
+  </si>
+  <si>
+    <t>vig_assign</t>
+  </si>
+  <si>
+    <t>vig_assign_tme_First Click</t>
+  </si>
+  <si>
+    <t>vig_assign_tme_Last Click</t>
+  </si>
+  <si>
+    <t>vig_assign_tme_Page Submit</t>
+  </si>
+  <si>
+    <t>vig_assign_tme_Click Count</t>
+  </si>
+  <si>
+    <t>PROLIFIC_PID</t>
+  </si>
+  <si>
+    <t>STUDY_ID</t>
+  </si>
+  <si>
+    <t>SESSION_ID</t>
+  </si>
+  <si>
+    <t>Question used to help assign vignettes to participants</t>
+  </si>
+  <si>
+    <t>For vig_assign display, timing of first click; can be ignored because screen auto proceeded after .01 seconds</t>
+  </si>
+  <si>
+    <t>always blank (screen should have only been shown for .1 seconds)</t>
+  </si>
+  <si>
+    <t>Same variable exists for vignette # 1 - 121 (Note: there are only 119 vignettes, but Qualtrics skipped the 2 and 3 numbering. This is inconsequential for how the data are processed)</t>
+  </si>
+  <si>
+    <t>Same variable exists for vignette # 1 - 121</t>
+  </si>
+  <si>
+    <t>Study  unique identifier</t>
+  </si>
+  <si>
+    <t>Session unique identifier</t>
   </si>
 </sst>
 </file>
@@ -1861,9 +1907,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1901,7 +1947,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2007,7 +2053,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2149,7 +2195,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2163,16 +2209,16 @@
       <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.25" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="13.8" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.42578125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="31.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.44140625" style="3" customWidth="1"/>
     <col min="3" max="3" width="60" style="3" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="8.7109375" style="3" hidden="1"/>
+    <col min="4" max="4" width="8.6640625" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="8.6640625" style="3" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2183,7 +2229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -2194,7 +2240,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>136</v>
       </c>
@@ -2205,7 +2251,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>137</v>
       </c>
@@ -2216,7 +2262,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>138</v>
       </c>
@@ -2227,7 +2273,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>139</v>
       </c>
@@ -2238,7 +2284,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>140</v>
       </c>
@@ -2249,7 +2295,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>141</v>
       </c>
@@ -2260,7 +2306,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -2271,7 +2317,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>142</v>
       </c>
@@ -2282,7 +2328,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>143</v>
       </c>
@@ -2293,7 +2339,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
@@ -2304,252 +2350,252 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
     </row>
-    <row r="25" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
     </row>
-    <row r="26" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
     </row>
-    <row r="27" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
     </row>
-    <row r="28" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
     </row>
-    <row r="29" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
     </row>
-    <row r="30" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
     </row>
-    <row r="31" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
     </row>
-    <row r="32" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
     </row>
-    <row r="33" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
     </row>
-    <row r="34" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
     </row>
-    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
     </row>
-    <row r="36" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
     </row>
-    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
     </row>
-    <row r="38" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
     </row>
-    <row r="39" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
     </row>
-    <row r="40" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
     </row>
-    <row r="41" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
     </row>
-    <row r="42" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
     </row>
-    <row r="43" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
     </row>
-    <row r="44" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
     </row>
-    <row r="45" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
     </row>
-    <row r="46" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
     </row>
-    <row r="47" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
     </row>
-    <row r="48" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
     </row>
-    <row r="49" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
     </row>
-    <row r="50" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
     </row>
-    <row r="51" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
     </row>
-    <row r="52" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
     </row>
-    <row r="53" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
     </row>
-    <row r="54" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
     </row>
-    <row r="55" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
     </row>
-    <row r="56" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
     </row>
-    <row r="57" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
     </row>
-    <row r="58" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
     </row>
-    <row r="59" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
     </row>
-    <row r="60" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
     </row>
-    <row r="61" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
     </row>
-    <row r="62" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -2568,18 +2614,18 @@
       <selection activeCell="B59" sqref="B59:C59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.42578125" customWidth="1"/>
-    <col min="3" max="3" width="40.85546875" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="31.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.44140625" customWidth="1"/>
+    <col min="3" max="3" width="40.88671875" customWidth="1"/>
+    <col min="4" max="4" width="23.44140625" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" customWidth="1"/>
     <col min="6" max="1210" width="0" hidden="1" customWidth="1"/>
-    <col min="1211" max="16384" width="8.7109375" hidden="1"/>
+    <col min="1211" max="16384" width="8.6640625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2593,7 +2639,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -2605,7 +2651,7 @@
       </c>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -2617,7 +2663,7 @@
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -2629,7 +2675,7 @@
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -2641,7 +2687,7 @@
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -2653,7 +2699,7 @@
       </c>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4" ht="29.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -2665,7 +2711,7 @@
       </c>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -2677,7 +2723,7 @@
       </c>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -2689,7 +2735,7 @@
       </c>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
@@ -2701,7 +2747,7 @@
       </c>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
@@ -2713,7 +2759,7 @@
       </c>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:4" ht="29.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -2727,7 +2773,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="29.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -2741,7 +2787,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="29.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
@@ -2755,7 +2801,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="29.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
@@ -2769,7 +2815,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="114.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="111" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
@@ -2783,7 +2829,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="157.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="153.6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>24</v>
       </c>
@@ -2797,7 +2843,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="129" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="126" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>25</v>
       </c>
@@ -2811,7 +2857,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="114.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="111.6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>26</v>
       </c>
@@ -2825,7 +2871,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="100.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="98.4" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>27</v>
       </c>
@@ -2839,7 +2885,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="43.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="42" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>28</v>
       </c>
@@ -2851,7 +2897,7 @@
       </c>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="1:4" ht="43.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="42" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>29</v>
       </c>
@@ -2863,7 +2909,7 @@
       </c>
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="1:4" ht="43.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="42" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>30</v>
       </c>
@@ -2875,7 +2921,7 @@
       </c>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4" ht="43.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="42" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>31</v>
       </c>
@@ -2887,7 +2933,7 @@
       </c>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:4" ht="143.25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="138.6" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>32</v>
       </c>
@@ -2901,7 +2947,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="143.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="138.6" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>33</v>
       </c>
@@ -2915,7 +2961,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="143.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="138.6" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>34</v>
       </c>
@@ -2929,7 +2975,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="143.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="138.6" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>35</v>
       </c>
@@ -2943,7 +2989,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="143.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="138.6" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>36</v>
       </c>
@@ -2957,7 +3003,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="143.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="138.6" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>37</v>
       </c>
@@ -2971,7 +3017,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="143.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="138.6" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>38</v>
       </c>
@@ -2985,7 +3031,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="143.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="138.6" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>39</v>
       </c>
@@ -2999,7 +3045,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="143.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="138.6" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>40</v>
       </c>
@@ -3013,7 +3059,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="143.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="138.6" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>41</v>
       </c>
@@ -3027,7 +3073,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="143.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="138.6" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>42</v>
       </c>
@@ -3041,7 +3087,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="143.25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="138.6" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>43</v>
       </c>
@@ -3055,7 +3101,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="143.25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="138.6" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>44</v>
       </c>
@@ -3069,7 +3115,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="143.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="138.6" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>45</v>
       </c>
@@ -3083,7 +3129,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="143.25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="138.6" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>46</v>
       </c>
@@ -3097,7 +3143,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="143.25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="138.6" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>47</v>
       </c>
@@ -3111,7 +3157,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="143.25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="138.6" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>48</v>
       </c>
@@ -3125,7 +3171,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="143.25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="138.6" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>49</v>
       </c>
@@ -3139,7 +3185,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="143.25" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="138.6" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>50</v>
       </c>
@@ -3153,7 +3199,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="143.25" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="138.6" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>51</v>
       </c>
@@ -3167,7 +3213,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="143.25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="138.6" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>52</v>
       </c>
@@ -3181,7 +3227,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="257.25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="221.4" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>53</v>
       </c>
@@ -3193,7 +3239,7 @@
       </c>
       <c r="D46" s="3"/>
     </row>
-    <row r="47" spans="1:4" ht="157.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="139.19999999999999" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>54</v>
       </c>
@@ -3205,7 +3251,7 @@
       </c>
       <c r="D47" s="3"/>
     </row>
-    <row r="48" spans="1:4" ht="157.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="125.4" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>55</v>
       </c>
@@ -3217,7 +3263,7 @@
       </c>
       <c r="D48" s="3"/>
     </row>
-    <row r="49" spans="1:4" ht="129" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="126" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>56</v>
       </c>
@@ -3229,7 +3275,7 @@
       </c>
       <c r="D49" s="3"/>
     </row>
-    <row r="50" spans="1:4" ht="100.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="98.4" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>57</v>
       </c>
@@ -3241,7 +3287,7 @@
       </c>
       <c r="D50" s="3"/>
     </row>
-    <row r="51" spans="1:4" ht="29.25" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>58</v>
       </c>
@@ -3253,7 +3299,7 @@
       </c>
       <c r="D51" s="3"/>
     </row>
-    <row r="52" spans="1:4" ht="29.25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>59</v>
       </c>
@@ -3265,7 +3311,7 @@
       </c>
       <c r="D52" s="3"/>
     </row>
-    <row r="53" spans="1:4" ht="43.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="42" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>60</v>
       </c>
@@ -3277,7 +3323,7 @@
       </c>
       <c r="D53" s="3"/>
     </row>
-    <row r="54" spans="1:4" ht="43.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" ht="42" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>61</v>
       </c>
@@ -3289,7 +3335,7 @@
       </c>
       <c r="D54" s="3"/>
     </row>
-    <row r="55" spans="1:4" ht="171.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" ht="167.4" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>62</v>
       </c>
@@ -3301,7 +3347,7 @@
       </c>
       <c r="D55" s="3"/>
     </row>
-    <row r="56" spans="1:4" ht="100.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" ht="97.2" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>63</v>
       </c>
@@ -3313,7 +3359,7 @@
       </c>
       <c r="D56" s="3"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>64</v>
       </c>
@@ -3325,7 +3371,7 @@
       </c>
       <c r="D57" s="3"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>65</v>
       </c>
@@ -3337,7 +3383,7 @@
       </c>
       <c r="D58" s="3"/>
     </row>
-    <row r="59" spans="1:4" ht="129" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" ht="124.8" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>66</v>
       </c>
@@ -3349,7 +3395,7 @@
       </c>
       <c r="D59" s="3"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>3</v>
       </c>
@@ -3361,7 +3407,7 @@
       </c>
       <c r="D60" s="3"/>
     </row>
-    <row r="61" spans="1:4" ht="43.5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" ht="42" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>67</v>
       </c>
@@ -3373,7 +3419,7 @@
       </c>
       <c r="D61" s="3"/>
     </row>
-    <row r="62" spans="1:4" ht="72" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" ht="69.599999999999994" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>68</v>
       </c>
@@ -3385,7 +3431,7 @@
       </c>
       <c r="D62" s="3"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3393,6 +3439,633 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C40C3E2-0206-4791-B58D-F77F179C5C9B}">
+  <dimension ref="A1:E67"/>
+  <sheetViews>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="31.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.44140625" customWidth="1"/>
+    <col min="3" max="3" width="40.88671875" customWidth="1"/>
+    <col min="4" max="4" width="23.44140625" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" customWidth="1"/>
+    <col min="6" max="16384" width="8.6640625" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="111" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="153.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="126" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="111.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="98.4" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:4" ht="42" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="1:4" ht="42" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:4" ht="167.4" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="1:4" ht="97.2" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" spans="1:4" ht="124.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="2"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" s="2"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" s="2"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+    </row>
+    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+    </row>
+    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+    </row>
+    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+    </row>
+    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+    </row>
+    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+    </row>
+    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+    </row>
+    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+    </row>
+    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+    </row>
+    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+    </row>
+    <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+    </row>
+    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+    </row>
+    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+    </row>
+    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="3"/>
+    </row>
+    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="2"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="3"/>
+    </row>
+    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="2"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="3"/>
+    </row>
+    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="2"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="3"/>
+    </row>
+    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="2"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="3"/>
+    </row>
+    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D56" s="3"/>
+    </row>
+    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D57" s="3"/>
+    </row>
+    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D58" s="3"/>
+    </row>
+    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D59" s="3"/>
+    </row>
+    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D60" s="3"/>
+    </row>
+    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D61" s="3"/>
+    </row>
+    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D62" s="3"/>
+    </row>
+    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D63" s="3"/>
+    </row>
+    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D64" s="3"/>
+    </row>
+    <row r="65" spans="4:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D65" s="3"/>
+    </row>
+    <row r="66" spans="4:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D66" s="3"/>
+    </row>
+    <row r="67" spans="4:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D67" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03407DD0-933A-466F-87CA-55DEA397E760}">
   <dimension ref="A1:D23"/>
   <sheetViews>
@@ -3400,16 +4073,16 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="143.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" hidden="1"/>
+    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="143.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -3420,7 +4093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>203</v>
       </c>
@@ -3431,7 +4104,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>204</v>
       </c>
@@ -3442,7 +4115,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>173</v>
       </c>
@@ -3453,7 +4126,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -3464,7 +4137,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>177</v>
       </c>
@@ -3475,7 +4148,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>179</v>
       </c>
@@ -3486,7 +4159,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="29.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>182</v>
       </c>
@@ -3497,7 +4170,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="57.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="55.8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>185</v>
       </c>
@@ -3508,7 +4181,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="43.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="42" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>188</v>
       </c>
@@ -3519,7 +4192,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="43.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="42" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>191</v>
       </c>
@@ -3530,7 +4203,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="29.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>194</v>
       </c>
@@ -3541,7 +4214,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="72" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="69.599999999999994" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>197</v>
       </c>
@@ -3552,7 +4225,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>200</v>
       </c>
@@ -3563,7 +4236,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>205</v>
       </c>
@@ -3574,7 +4247,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="43.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>206</v>
       </c>
@@ -3585,7 +4258,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>207</v>
       </c>
@@ -3596,7 +4269,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>208</v>
       </c>
@@ -3607,7 +4280,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>54</v>
       </c>
@@ -3618,7 +4291,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>57</v>
       </c>
@@ -3629,7 +4302,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>56</v>
       </c>
@@ -3640,7 +4313,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>55</v>
       </c>
@@ -3651,31 +4324,31 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B27CBC70-28B0-4D99-9FAB-33D140B18F6E}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C12" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="77.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="7" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="7" hidden="1"/>
+    <col min="1" max="1" width="14.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="77.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" style="7" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="7" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -3686,7 +4359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>219</v>
       </c>
@@ -3697,7 +4370,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>67</v>
       </c>
@@ -3708,7 +4381,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>220</v>
       </c>
@@ -3719,7 +4392,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>221</v>
       </c>
@@ -3730,7 +4403,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>222</v>
       </c>
@@ -3741,7 +4414,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>223</v>
       </c>
@@ -3752,7 +4425,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>224</v>
       </c>
@@ -3763,7 +4436,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="129" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="126" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>54</v>
       </c>
@@ -3774,7 +4447,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="129" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="111.6" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>55</v>
       </c>
@@ -3785,7 +4458,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="100.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="97.8" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>56</v>
       </c>
@@ -3796,7 +4469,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="72" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="70.2" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>57</v>
       </c>
@@ -3807,7 +4480,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="129" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="126" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>62</v>
       </c>
@@ -3818,7 +4491,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="86.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="83.4" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>63</v>
       </c>
@@ -3829,7 +4502,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>65</v>
       </c>
@@ -3840,7 +4513,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="114.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="97.2" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>66</v>
       </c>
@@ -3851,7 +4524,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>225</v>
       </c>
@@ -3862,7 +4535,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>226</v>
       </c>
@@ -3873,7 +4546,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>227</v>
       </c>

</xml_diff>

<commit_message>
Code and file clean up
</commit_message>
<xml_diff>
--- a/data/metaware_csv_codebooks.xlsx
+++ b/data/metaware_csv_codebooks.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ncole\Documents\GitHub\metaware\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18790ADE-9169-4F34-820F-667278FE2C6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF9A17E1-CAEA-4826-898F-05FBA86FFD5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metaware_VigCombined.csv" sheetId="3" r:id="rId1"/>
     <sheet name="metaware_SurvData_raw.csv" sheetId="2" r:id="rId2"/>
     <sheet name="metaware_SurvData2_raw.csv " sheetId="6" r:id="rId3"/>
-    <sheet name="metaware_meta_clean.csv" sheetId="4" r:id="rId4"/>
-    <sheet name="metaware_replication_clean.csv" sheetId="5" r:id="rId5"/>
+    <sheet name="metaware_EsData_raw.xlsx" sheetId="7" r:id="rId4"/>
+    <sheet name="metaware_meta_clean.csv" sheetId="4" r:id="rId5"/>
+    <sheet name="metaware_replication_clean.csv" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="269">
   <si>
     <t>Variable</t>
   </si>
@@ -1142,12 +1143,6 @@
 double = comparison group is another demand condition</t>
   </si>
   <si>
-    <t>Cohen's d estimate</t>
-  </si>
-  <si>
-    <t>Cohen's d variability estimate</t>
-  </si>
-  <si>
     <t>Rated motivation to provide hypothesis-consistent responses</t>
   </si>
   <si>
@@ -1290,6 +1285,45 @@
   </si>
   <si>
     <t>Session unique identifier</t>
+  </si>
+  <si>
+    <t>lb</t>
+  </si>
+  <si>
+    <t>ub</t>
+  </si>
+  <si>
+    <t>report</t>
+  </si>
+  <si>
+    <t>external</t>
+  </si>
+  <si>
+    <t>internal</t>
+  </si>
+  <si>
+    <t>Average rating of reporting quality from modified Downs and Black checklist (higher = better)</t>
+  </si>
+  <si>
+    <t>Average rating of external validity from modified Downs and Black checklist (higher = better)</t>
+  </si>
+  <si>
+    <t>Average rating of internal validity from modified Downs and Black checklist (higher = better)</t>
+  </si>
+  <si>
+    <t>Codebooks are in located in the Excel file</t>
+  </si>
+  <si>
+    <t>Hedge's g estimate</t>
+  </si>
+  <si>
+    <t>Hedge's g variability estimate</t>
+  </si>
+  <si>
+    <t>95% CI lower bound of Hedge's g estimate</t>
+  </si>
+  <si>
+    <t>95% CI upper bound of Hedge's g estimate</t>
   </si>
 </sst>
 </file>
@@ -3442,7 +3476,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C40C3E2-0206-4791-B58D-F77F179C5C9B}">
   <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="F1" sqref="F1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -3592,21 +3626,21 @@
     </row>
     <row r="12" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>251</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>6</v>
@@ -3614,10 +3648,10 @@
     </row>
     <row r="14" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>6</v>
@@ -3625,10 +3659,10 @@
     </row>
     <row r="15" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>6</v>
@@ -3636,10 +3670,10 @@
     </row>
     <row r="16" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>6</v>
@@ -3740,7 +3774,7 @@
         <v>159</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="111.6" x14ac:dyDescent="0.3">
@@ -3754,7 +3788,7 @@
         <v>160</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="98.4" x14ac:dyDescent="0.3">
@@ -3768,7 +3802,7 @@
         <v>162</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
@@ -3881,7 +3915,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>132</v>
@@ -3893,10 +3927,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>5</v>
@@ -3905,10 +3939,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>5</v>
@@ -4066,11 +4100,35 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54B9CC17-FE1A-4E6C-AB3A-ECA373D2FA29}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="38.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="1.88671875" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03407DD0-933A-466F-87CA-55DEA397E760}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
@@ -4263,7 +4321,7 @@
         <v>207</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>213</v>
+        <v>265</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>6</v>
@@ -4274,7 +4332,7 @@
         <v>208</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>214</v>
+        <v>266</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>6</v>
@@ -4282,10 +4340,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>54</v>
+        <v>256</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>215</v>
+        <v>267</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>6</v>
@@ -4293,10 +4351,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>57</v>
+        <v>257</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>216</v>
+        <v>268</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>6</v>
@@ -4304,10 +4362,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>6</v>
@@ -4315,28 +4373,82 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3"/>
+      <c r="B24" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B27CBC70-28B0-4D99-9FAB-33D140B18F6E}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4360,84 +4472,84 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>219</v>
+      <c r="A2" s="2" t="s">
+        <v>217</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:3" ht="42" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:3" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="B6" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C5" s="7" t="s">
+      <c r="B7" s="2" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="C7" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="B7" s="7" t="s">
+      <c r="B8" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C8" s="2" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
-        <v>224</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>237</v>
-      </c>
-    </row>
     <row r="9" spans="1:3" ht="126" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -4448,7 +4560,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="111.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -4459,7 +4571,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="97.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -4470,7 +4582,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="70.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -4481,7 +4593,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="126" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -4492,18 +4604,18 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="83.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>126</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="2" t="s">
         <v>65</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -4514,46 +4626,46 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="97.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>130</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B19" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>239</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
-        <v>227</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="2" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added comparison to the workflow
</commit_message>
<xml_diff>
--- a/data/metaware_csv_codebooks.xlsx
+++ b/data/metaware_csv_codebooks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ncole\Documents\GitHub\metaware\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ncoles/Documents/GitHub/metaware/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF9A17E1-CAEA-4826-898F-05FBA86FFD5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5991BC2D-FBDE-1945-A071-65184F7435D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12460" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metaware_VigCombined.csv" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="272">
   <si>
     <t>Variable</t>
   </si>
@@ -1324,6 +1324,16 @@
   </si>
   <si>
     <t>95% CI upper bound of Hedge's g estimate</t>
+  </si>
+  <si>
+    <t>comparison</t>
+  </si>
+  <si>
+    <t>Indicator of whether effect size is indicative of a difference or difference-in-difference</t>
+  </si>
+  <si>
+    <t>diff = difference 
+diff_diff = difference in difference</t>
   </si>
 </sst>
 </file>
@@ -2243,16 +2253,16 @@
       <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="13.8" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14" zeroHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.44140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="31.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.5" style="3" customWidth="1"/>
     <col min="3" max="3" width="60" style="3" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" style="3" customWidth="1"/>
     <col min="5" max="16384" width="8.6640625" style="3" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2263,7 +2273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -2274,7 +2284,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>136</v>
       </c>
@@ -2285,7 +2295,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>137</v>
       </c>
@@ -2296,7 +2306,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
         <v>138</v>
       </c>
@@ -2307,7 +2317,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
         <v>139</v>
       </c>
@@ -2318,7 +2328,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
         <v>140</v>
       </c>
@@ -2329,7 +2339,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
         <v>141</v>
       </c>
@@ -2340,7 +2350,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -2351,7 +2361,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
         <v>142</v>
       </c>
@@ -2362,7 +2372,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
         <v>143</v>
       </c>
@@ -2373,7 +2383,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
@@ -2384,252 +2394,252 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
     </row>
-    <row r="25" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
     </row>
-    <row r="26" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
     </row>
-    <row r="27" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
     </row>
-    <row r="28" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
     </row>
-    <row r="29" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
     </row>
-    <row r="30" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
     </row>
-    <row r="31" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
     </row>
-    <row r="32" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
     </row>
-    <row r="33" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
     </row>
-    <row r="34" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
     </row>
-    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
     </row>
-    <row r="36" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
     </row>
-    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
     </row>
-    <row r="38" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
     </row>
-    <row r="39" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
     </row>
-    <row r="40" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
     </row>
-    <row r="41" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
     </row>
-    <row r="42" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
     </row>
-    <row r="43" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
     </row>
-    <row r="44" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
     </row>
-    <row r="45" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
     </row>
-    <row r="46" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
     </row>
-    <row r="47" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
     </row>
-    <row r="48" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
     </row>
-    <row r="49" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
     </row>
-    <row r="50" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
     </row>
-    <row r="51" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
     </row>
-    <row r="52" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
     </row>
-    <row r="53" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
     </row>
-    <row r="54" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
     </row>
-    <row r="55" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
     </row>
-    <row r="56" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
     </row>
-    <row r="57" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
     </row>
-    <row r="58" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
     </row>
-    <row r="59" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
     </row>
-    <row r="60" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
     </row>
-    <row r="61" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
     </row>
-    <row r="62" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" hidden="1" x14ac:dyDescent="0.15">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -2648,18 +2658,18 @@
       <selection activeCell="B59" sqref="B59:C59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.44140625" customWidth="1"/>
-    <col min="3" max="3" width="40.88671875" customWidth="1"/>
-    <col min="4" max="4" width="23.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.5" customWidth="1"/>
+    <col min="3" max="3" width="40.83203125" customWidth="1"/>
+    <col min="4" max="4" width="23.5" customWidth="1"/>
     <col min="5" max="5" width="8.6640625" customWidth="1"/>
     <col min="6" max="1210" width="0" hidden="1" customWidth="1"/>
     <col min="1211" max="16384" width="8.6640625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2673,7 +2683,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -2685,7 +2695,7 @@
       </c>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -2697,7 +2707,7 @@
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -2709,7 +2719,7 @@
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -2721,7 +2731,7 @@
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -2733,7 +2743,7 @@
       </c>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="31" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -2745,7 +2755,7 @@
       </c>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -2757,7 +2767,7 @@
       </c>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -2769,7 +2779,7 @@
       </c>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
@@ -2781,7 +2791,7 @@
       </c>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
@@ -2793,7 +2803,7 @@
       </c>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="31" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -2807,7 +2817,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="31" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -2821,7 +2831,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="31" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
@@ -2835,7 +2845,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="31" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
@@ -2849,7 +2859,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="111" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="106" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
@@ -2863,7 +2873,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="153.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="166" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>24</v>
       </c>
@@ -2877,7 +2887,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="126" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>25</v>
       </c>
@@ -2891,7 +2901,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="111.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="106" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>26</v>
       </c>
@@ -2905,7 +2915,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="98.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="106" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>27</v>
       </c>
@@ -2919,7 +2929,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="42" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="46" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>28</v>
       </c>
@@ -2931,7 +2941,7 @@
       </c>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="1:4" ht="42" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="46" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>29</v>
       </c>
@@ -2943,7 +2953,7 @@
       </c>
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="1:4" ht="42" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="46" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>30</v>
       </c>
@@ -2955,7 +2965,7 @@
       </c>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4" ht="42" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="46" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>31</v>
       </c>
@@ -2967,7 +2977,7 @@
       </c>
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="1:4" ht="138.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>32</v>
       </c>
@@ -2981,7 +2991,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="138.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>33</v>
       </c>
@@ -2995,7 +3005,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="138.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>34</v>
       </c>
@@ -3009,7 +3019,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="138.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>35</v>
       </c>
@@ -3023,7 +3033,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="138.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>36</v>
       </c>
@@ -3037,7 +3047,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="138.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>37</v>
       </c>
@@ -3051,7 +3061,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="138.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>38</v>
       </c>
@@ -3065,7 +3075,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="138.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>39</v>
       </c>
@@ -3079,7 +3089,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="138.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>40</v>
       </c>
@@ -3093,7 +3103,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="138.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>41</v>
       </c>
@@ -3107,7 +3117,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="138.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>42</v>
       </c>
@@ -3121,7 +3131,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="138.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>43</v>
       </c>
@@ -3135,7 +3145,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="138.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>44</v>
       </c>
@@ -3149,7 +3159,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="138.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>45</v>
       </c>
@@ -3163,7 +3173,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="138.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>46</v>
       </c>
@@ -3177,7 +3187,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="138.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>47</v>
       </c>
@@ -3191,7 +3201,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="138.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>48</v>
       </c>
@@ -3205,7 +3215,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="138.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>49</v>
       </c>
@@ -3219,7 +3229,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="138.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>50</v>
       </c>
@@ -3233,7 +3243,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="138.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>51</v>
       </c>
@@ -3247,7 +3257,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="138.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>52</v>
       </c>
@@ -3261,7 +3271,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="221.4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" ht="226" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>53</v>
       </c>
@@ -3273,7 +3283,7 @@
       </c>
       <c r="D46" s="3"/>
     </row>
-    <row r="47" spans="1:4" ht="139.19999999999999" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>54</v>
       </c>
@@ -3285,7 +3295,7 @@
       </c>
       <c r="D47" s="3"/>
     </row>
-    <row r="48" spans="1:4" ht="125.4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>55</v>
       </c>
@@ -3297,7 +3307,7 @@
       </c>
       <c r="D48" s="3"/>
     </row>
-    <row r="49" spans="1:4" ht="126" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>56</v>
       </c>
@@ -3309,7 +3319,7 @@
       </c>
       <c r="D49" s="3"/>
     </row>
-    <row r="50" spans="1:4" ht="98.4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" ht="106" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>57</v>
       </c>
@@ -3321,7 +3331,7 @@
       </c>
       <c r="D50" s="3"/>
     </row>
-    <row r="51" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" ht="31" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>58</v>
       </c>
@@ -3333,7 +3343,7 @@
       </c>
       <c r="D51" s="3"/>
     </row>
-    <row r="52" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" ht="31" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>59</v>
       </c>
@@ -3345,7 +3355,7 @@
       </c>
       <c r="D52" s="3"/>
     </row>
-    <row r="53" spans="1:4" ht="42" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" ht="46" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>60</v>
       </c>
@@ -3357,7 +3367,7 @@
       </c>
       <c r="D53" s="3"/>
     </row>
-    <row r="54" spans="1:4" ht="42" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" ht="46" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>61</v>
       </c>
@@ -3369,7 +3379,7 @@
       </c>
       <c r="D54" s="3"/>
     </row>
-    <row r="55" spans="1:4" ht="167.4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" ht="181" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>62</v>
       </c>
@@ -3381,7 +3391,7 @@
       </c>
       <c r="D55" s="3"/>
     </row>
-    <row r="56" spans="1:4" ht="97.2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" ht="106" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>63</v>
       </c>
@@ -3393,7 +3403,7 @@
       </c>
       <c r="D56" s="3"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>64</v>
       </c>
@@ -3405,7 +3415,7 @@
       </c>
       <c r="D57" s="3"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>65</v>
       </c>
@@ -3417,7 +3427,7 @@
       </c>
       <c r="D58" s="3"/>
     </row>
-    <row r="59" spans="1:4" ht="124.8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" ht="121" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>66</v>
       </c>
@@ -3429,7 +3439,7 @@
       </c>
       <c r="D59" s="3"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>3</v>
       </c>
@@ -3441,7 +3451,7 @@
       </c>
       <c r="D60" s="3"/>
     </row>
-    <row r="61" spans="1:4" ht="42" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" ht="46" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>67</v>
       </c>
@@ -3453,7 +3463,7 @@
       </c>
       <c r="D61" s="3"/>
     </row>
-    <row r="62" spans="1:4" ht="69.599999999999994" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" ht="76" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>68</v>
       </c>
@@ -3465,7 +3475,7 @@
       </c>
       <c r="D62" s="3"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3"/>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3480,17 +3490,17 @@
       <selection activeCell="F1" sqref="F1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.44140625" customWidth="1"/>
-    <col min="3" max="3" width="40.88671875" customWidth="1"/>
-    <col min="4" max="4" width="23.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.5" customWidth="1"/>
+    <col min="3" max="3" width="40.83203125" customWidth="1"/>
+    <col min="4" max="4" width="23.5" customWidth="1"/>
     <col min="5" max="5" width="8.6640625" customWidth="1"/>
     <col min="6" max="16384" width="8.6640625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3504,7 +3514,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -3516,7 +3526,7 @@
       </c>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -3528,7 +3538,7 @@
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -3540,7 +3550,7 @@
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -3552,7 +3562,7 @@
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -3564,7 +3574,7 @@
       </c>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="31" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -3576,7 +3586,7 @@
       </c>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -3588,7 +3598,7 @@
       </c>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -3600,7 +3610,7 @@
       </c>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
@@ -3612,7 +3622,7 @@
       </c>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
@@ -3624,7 +3634,7 @@
       </c>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="31" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>241</v>
       </c>
@@ -3635,7 +3645,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="31" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>242</v>
       </c>
@@ -3646,7 +3656,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="31" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>243</v>
       </c>
@@ -3657,7 +3667,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="31" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>244</v>
       </c>
@@ -3668,7 +3678,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="31" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>245</v>
       </c>
@@ -3679,7 +3689,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="31" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>19</v>
       </c>
@@ -3693,7 +3703,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="31" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>20</v>
       </c>
@@ -3707,7 +3717,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="31" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>21</v>
       </c>
@@ -3721,7 +3731,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="31" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>22</v>
       </c>
@@ -3735,7 +3745,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="111" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="106" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>23</v>
       </c>
@@ -3749,7 +3759,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="153.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="166" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>24</v>
       </c>
@@ -3763,7 +3773,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="126" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>25</v>
       </c>
@@ -3777,7 +3787,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="111.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="106" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>26</v>
       </c>
@@ -3791,7 +3801,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="98.4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="106" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>27</v>
       </c>
@@ -3805,7 +3815,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="31" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>58</v>
       </c>
@@ -3817,7 +3827,7 @@
       </c>
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="31" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>59</v>
       </c>
@@ -3829,7 +3839,7 @@
       </c>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4" ht="42" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="46" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>60</v>
       </c>
@@ -3841,7 +3851,7 @@
       </c>
       <c r="D28" s="3"/>
     </row>
-    <row r="29" spans="1:4" ht="42" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="46" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>61</v>
       </c>
@@ -3853,7 +3863,7 @@
       </c>
       <c r="D29" s="3"/>
     </row>
-    <row r="30" spans="1:4" ht="167.4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="181" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>62</v>
       </c>
@@ -3865,7 +3875,7 @@
       </c>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="1:4" ht="97.2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="106" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>63</v>
       </c>
@@ -3877,7 +3887,7 @@
       </c>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>64</v>
       </c>
@@ -3889,7 +3899,7 @@
       </c>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>65</v>
       </c>
@@ -3901,7 +3911,7 @@
       </c>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="1:4" ht="124.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="121" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>66</v>
       </c>
@@ -3913,7 +3923,7 @@
       </c>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>246</v>
       </c>
@@ -3925,7 +3935,7 @@
       </c>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>247</v>
       </c>
@@ -3937,7 +3947,7 @@
       </c>
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>248</v>
       </c>
@@ -3949,148 +3959,148 @@
       </c>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
     </row>
-    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
     </row>
-    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
     </row>
-    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
     </row>
-    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
     </row>
-    <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
     </row>
-    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
     </row>
-    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
     </row>
-    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="3"/>
     </row>
-    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="3"/>
     </row>
-    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="3"/>
     </row>
-    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="3"/>
     </row>
-    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="3"/>
     </row>
-    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="D56" s="3"/>
     </row>
-    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="D57" s="3"/>
     </row>
-    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="D58" s="3"/>
     </row>
-    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="D59" s="3"/>
     </row>
-    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="D60" s="3"/>
     </row>
-    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="D61" s="3"/>
     </row>
-    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="D62" s="3"/>
     </row>
-    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="D63" s="3"/>
     </row>
-    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="D64" s="3"/>
     </row>
-    <row r="65" spans="4:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="4:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="D65" s="3"/>
     </row>
-    <row r="66" spans="4:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="4:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="D66" s="3"/>
     </row>
-    <row r="67" spans="4:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="4:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="D67" s="3"/>
     </row>
   </sheetData>
@@ -4105,19 +4115,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="38.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="1.88671875" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" hidden="1"/>
+    <col min="2" max="2" width="1.83203125" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:1" ht="10.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4125,22 +4135,22 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03407DD0-933A-466F-87CA-55DEA397E760}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="143.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" hidden="1"/>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="143.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" customWidth="1"/>
+    <col min="5" max="16384" width="9.1640625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -4151,7 +4161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>203</v>
       </c>
@@ -4162,7 +4172,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>204</v>
       </c>
@@ -4173,7 +4183,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>173</v>
       </c>
@@ -4184,7 +4194,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -4195,7 +4205,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>177</v>
       </c>
@@ -4206,7 +4216,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>179</v>
       </c>
@@ -4217,7 +4227,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="31" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>182</v>
       </c>
@@ -4228,7 +4238,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="55.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="61" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>185</v>
       </c>
@@ -4239,7 +4249,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="42" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="46" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>188</v>
       </c>
@@ -4250,7 +4260,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="42" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="46" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>191</v>
       </c>
@@ -4261,7 +4271,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="31" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>194</v>
       </c>
@@ -4272,7 +4282,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="69.599999999999994" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="76" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>197</v>
       </c>
@@ -4283,7 +4293,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>200</v>
       </c>
@@ -4294,7 +4304,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>205</v>
       </c>
@@ -4305,135 +4315,146 @@
         <v>210</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="31" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="31" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+      <c r="C18" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
+      <c r="C19" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
+      <c r="C20" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="C20" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
+      <c r="C21" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
+      <c r="C22" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="C22" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
+      <c r="C23" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
+      <c r="C24" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
+      <c r="C25" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
+      <c r="C26" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="C26" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
+      <c r="C27" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C28" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -4451,16 +4472,16 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.6640625" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="70.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="77.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" style="7" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="7" hidden="1"/>
+    <col min="3" max="3" width="77.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" style="7" customWidth="1"/>
+    <col min="5" max="16384" width="9.1640625" style="7" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -4471,7 +4492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>217</v>
       </c>
@@ -4482,7 +4503,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="42" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="46" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>67</v>
       </c>
@@ -4493,7 +4514,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="31" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>218</v>
       </c>
@@ -4504,7 +4525,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="31" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>219</v>
       </c>
@@ -4515,7 +4536,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>220</v>
       </c>
@@ -4526,7 +4547,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="31" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>221</v>
       </c>
@@ -4537,7 +4558,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="31" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>222</v>
       </c>
@@ -4548,7 +4569,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="126" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="106" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>54</v>
       </c>
@@ -4559,7 +4580,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="111.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="106" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>55</v>
       </c>
@@ -4570,7 +4591,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="97.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="106" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>56</v>
       </c>
@@ -4581,7 +4602,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="70.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="76" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>57</v>
       </c>
@@ -4592,7 +4613,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="126" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="136" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>62</v>
       </c>
@@ -4603,7 +4624,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="83.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="91" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>63</v>
       </c>
@@ -4614,7 +4635,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>65</v>
       </c>
@@ -4625,7 +4646,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="97.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="106" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>66</v>
       </c>
@@ -4636,7 +4657,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>223</v>
       </c>
@@ -4647,7 +4668,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>224</v>
       </c>
@@ -4658,7 +4679,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>225</v>
       </c>

</xml_diff>

<commit_message>
ADDED NA'S TO DATAFILE
</commit_message>
<xml_diff>
--- a/data/metaware_csv_codebooks.xlsx
+++ b/data/metaware_csv_codebooks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ncoles/Documents/GitHub/metaware/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5991BC2D-FBDE-1945-A071-65184F7435D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A13587F4-A38C-AF47-B260-9569C621B9C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12460" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="140" yWindow="660" windowWidth="31680" windowHeight="17180" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metaware_VigCombined.csv" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="275">
   <si>
     <t>Variable</t>
   </si>
@@ -1334,6 +1334,15 @@
   <si>
     <t>diff = difference 
 diff_diff = difference in difference</t>
+  </si>
+  <si>
+    <t>county</t>
+  </si>
+  <si>
+    <t>Indicator of what country the investigation was conducted in (or, if not stated, the country of the corresponding author)</t>
+  </si>
+  <si>
+    <t>coded according to ISO-3 standards</t>
   </si>
 </sst>
 </file>
@@ -4135,10 +4144,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03407DD0-933A-466F-87CA-55DEA397E760}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -4238,122 +4247,122 @@
         <v>184</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="61" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="61" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C10" s="5" t="s">
         <v>187</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="46" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="46" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="46" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C12" s="5" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="31" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+    <row r="13" spans="1:3" ht="31" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C13" s="5" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="76" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+    <row r="14" spans="1:3" ht="76" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C14" s="6" t="s">
         <v>199</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C16" s="5" t="s">
         <v>210</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="31" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="31" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="31" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>212</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>6</v>
@@ -4361,10 +4370,10 @@
     </row>
     <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>256</v>
+        <v>208</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>6</v>
@@ -4372,10 +4381,10 @@
     </row>
     <row r="21" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>6</v>
@@ -4383,10 +4392,10 @@
     </row>
     <row r="22" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>54</v>
+        <v>257</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>213</v>
+        <v>268</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>6</v>
@@ -4394,10 +4403,10 @@
     </row>
     <row r="23" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>6</v>
@@ -4405,10 +4414,10 @@
     </row>
     <row r="24" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>6</v>
@@ -4416,10 +4425,10 @@
     </row>
     <row r="25" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>6</v>
@@ -4427,10 +4436,10 @@
     </row>
     <row r="26" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>258</v>
+        <v>55</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>261</v>
+        <v>216</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>6</v>
@@ -4438,10 +4447,10 @@
     </row>
     <row r="27" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>6</v>
@@ -4449,12 +4458,23 @@
     </row>
     <row r="28" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C29" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -4468,7 +4488,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B27CBC70-28B0-4D99-9FAB-33D140B18F6E}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>